<commit_message>
Added comments about meaning of the rows and columns of the data.
</commit_message>
<xml_diff>
--- a/docs/CalculationSpeedAnalysis.xlsx
+++ b/docs/CalculationSpeedAnalysis.xlsx
@@ -5,22 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bin\mrakitin\sirepo_benchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bin\mrakitin\sirepo_benchmark\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" tabRatio="654" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1. Web v Command line User Time" sheetId="2" r:id="rId1"/>
     <sheet name="2. Web v CL calculation time" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="3. Servers Speeds Comparison" sheetId="3" r:id="rId4"/>
-    <sheet name="Server preparation time" sheetId="6" r:id="rId5"/>
-    <sheet name="1. Short version" sheetId="4" r:id="rId6"/>
+    <sheet name="3. Servers Speeds Comparison" sheetId="3" r:id="rId3"/>
+    <sheet name="Server preparation time" sheetId="6" r:id="rId4"/>
+    <sheet name="1. Short version" sheetId="4" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
   <si>
     <t>Calculation time comparisons between web and command line interfaces</t>
   </si>
@@ -143,6 +142,9 @@
   </si>
   <si>
     <t>Standard deviation:</t>
+  </si>
+  <si>
+    <t>total - waiting (s)</t>
   </si>
 </sst>
 </file>
@@ -385,7 +387,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,6 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
@@ -4906,6 +4909,66 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>524830</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC932652-FFF8-4A4E-9E74-9EC314781D46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="3977" t="10539" r="9078" b="6690"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11534774" y="200025"/>
+          <a:ext cx="8411531" cy="5629275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -5362,7 +5425,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5382,10 +5445,10 @@
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="25"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1">
@@ -6127,7 +6190,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6142,15 +6205,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -6162,10 +6225,10 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="29"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
@@ -6347,13 +6410,13 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6368,27 +6431,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40:G40"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6403,15 +6449,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -6476,10 +6522,10 @@
       <c r="E7">
         <v>6.94</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="31"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:7">
       <c r="D8" s="8">
@@ -6552,10 +6598,10 @@
       <c r="E13">
         <v>36.24</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="31"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:7">
       <c r="D14" s="8">
@@ -6634,10 +6680,10 @@
       <c r="E20">
         <v>9.09</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" spans="1:7">
       <c r="D21" s="8">
@@ -6710,10 +6756,10 @@
       <c r="E26">
         <v>42.26</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="31"/>
+      <c r="G26" s="32"/>
     </row>
     <row r="27" spans="1:7">
       <c r="D27" s="8">
@@ -6792,10 +6838,10 @@
       <c r="E33">
         <v>6.7</v>
       </c>
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="31"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" spans="3:7">
       <c r="D34" s="8">
@@ -6868,10 +6914,10 @@
       <c r="E40">
         <v>31.61</v>
       </c>
-      <c r="F40" s="31" t="s">
+      <c r="F40" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="31"/>
+      <c r="G40" s="32"/>
     </row>
     <row r="41" spans="3:7">
       <c r="D41" s="8">
@@ -6925,12 +6971,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6945,7 +6991,7 @@
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -6967,8 +7013,11 @@
       <c r="G1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -6993,7 +7042,7 @@
         <v>0.14013497419610954</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="C3">
         <v>15.2</v>
       </c>
@@ -7012,7 +7061,7 @@
         <v>0.17558779389694848</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="C4">
         <v>14.76</v>
       </c>
@@ -7031,7 +7080,7 @@
         <v>0.15236567762630307</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="C5">
         <v>14.91</v>
       </c>
@@ -7050,7 +7099,7 @@
         <v>0.13282001924927814</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="C6">
         <v>14.55</v>
       </c>
@@ -7069,7 +7118,7 @@
         <v>0.17227523857358118</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="C7" s="9">
         <f>AVERAGE(C2:C6)</f>
         <v>15.017999999999997</v>
@@ -7093,8 +7142,12 @@
       <c r="H7" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I7" s="24">
+        <f>F7-C7</f>
+        <v>7.1440000000000019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -7119,7 +7172,7 @@
         <v>9.6852300242130762E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="C10">
         <v>11.66</v>
       </c>
@@ -7138,7 +7191,7 @@
         <v>0.11056207535515755</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="C11">
         <v>12.29</v>
       </c>
@@ -7157,7 +7210,7 @@
         <v>0.10520023909145247</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="C12">
         <v>12.45</v>
       </c>
@@ -7176,7 +7229,7 @@
         <v>0.10354857475276319</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="C13">
         <v>11.98</v>
       </c>
@@ -7195,7 +7248,7 @@
         <v>0.10995723885155777</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="C14" s="9">
         <f>AVERAGE(C9:C13)</f>
         <v>12.136000000000001</v>
@@ -7219,8 +7272,12 @@
       <c r="H14" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I14" s="24">
+        <f>F14-C14</f>
+        <v>5.2900000000000009</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -7245,7 +7302,7 @@
         <v>0.11502590673575132</v>
       </c>
     </row>
-    <row r="17" spans="3:8">
+    <row r="17" spans="3:9">
       <c r="C17">
         <v>15.86</v>
       </c>
@@ -7264,7 +7321,7 @@
         <v>0.10717948717948718</v>
       </c>
     </row>
-    <row r="18" spans="3:8">
+    <row r="18" spans="3:9">
       <c r="C18">
         <v>16.010000000000002</v>
       </c>
@@ -7283,7 +7340,7 @@
         <v>0.13880445795339424</v>
       </c>
     </row>
-    <row r="19" spans="3:8">
+    <row r="19" spans="3:9">
       <c r="C19">
         <v>16.440000000000001</v>
       </c>
@@ -7302,7 +7359,7 @@
         <v>0.11199207135778005</v>
       </c>
     </row>
-    <row r="20" spans="3:8">
+    <row r="20" spans="3:9">
       <c r="C20">
         <v>15.88</v>
       </c>
@@ -7321,7 +7378,7 @@
         <v>0.10410256410256416</v>
       </c>
     </row>
-    <row r="21" spans="3:8">
+    <row r="21" spans="3:9">
       <c r="C21" s="9">
         <f>AVERAGE(C16:C20)</f>
         <v>15.917999999999997</v>
@@ -7345,19 +7402,24 @@
       <c r="H21" s="9" t="s">
         <v>33</v>
       </c>
+      <c r="I21">
+        <f>F21-C21</f>
+        <v>3.7260000000000009</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7378,10 +7440,10 @@
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="25"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1">

</xml_diff>